<commit_message>
Added the pre-processed Spending algorithm
</commit_message>
<xml_diff>
--- a/Python/Result1.xlsx
+++ b/Python/Result1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,13 +504,13 @@
         <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>0.050425</v>
+        <v>0.053954</v>
       </c>
       <c r="E2" t="n">
         <v>1390</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01114</v>
+        <v>9.695</v>
       </c>
       <c r="G2" t="n">
         <v>10</v>
@@ -519,22 +519,22 @@
         <v>5.1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002966</v>
+        <v>2.8614</v>
       </c>
       <c r="J2" t="n">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="K2" t="n">
-        <v>0.15205</v>
+        <v>0.1495915</v>
       </c>
       <c r="L2" t="n">
-        <v>5554</v>
+        <v>5.554</v>
       </c>
       <c r="M2" t="n">
-        <v>0.172362</v>
+        <v>0.1697735</v>
       </c>
       <c r="N2" t="n">
-        <v>0.000148</v>
+        <v>0.000121</v>
       </c>
     </row>
     <row r="3">
@@ -548,13 +548,13 @@
         <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>0.052951</v>
+        <v>0.052513</v>
       </c>
       <c r="E3" t="n">
         <v>1390</v>
       </c>
       <c r="F3" t="n">
-        <v>0.019302</v>
+        <v>18.4481</v>
       </c>
       <c r="G3" t="n">
         <v>20</v>
@@ -563,22 +563,22 @@
         <v>10.1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.005628</v>
+        <v>5.173999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>14.4</v>
+        <v>144</v>
       </c>
       <c r="K3" t="n">
-        <v>0.187161</v>
+        <v>0.1876047</v>
       </c>
       <c r="L3" t="n">
-        <v>5556</v>
+        <v>5.556</v>
       </c>
       <c r="M3" t="n">
-        <v>0.179755</v>
+        <v>0.1788506</v>
       </c>
       <c r="N3" t="n">
-        <v>5.3e-05</v>
+        <v>5.9e-05</v>
       </c>
     </row>
     <row r="4">
@@ -592,13 +592,13 @@
         <v>150</v>
       </c>
       <c r="D4" t="n">
-        <v>0.054525</v>
+        <v>0.052353</v>
       </c>
       <c r="E4" t="n">
         <v>1390</v>
       </c>
       <c r="F4" t="n">
-        <v>0.027286</v>
+        <v>26.8248</v>
       </c>
       <c r="G4" t="n">
         <v>30</v>
@@ -607,22 +607,22 @@
         <v>15.1</v>
       </c>
       <c r="I4" t="n">
-        <v>0.007649</v>
+        <v>7.597799999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>14.8</v>
+        <v>148</v>
       </c>
       <c r="K4" t="n">
-        <v>0.226148</v>
+        <v>0.2233237</v>
       </c>
       <c r="L4" t="n">
-        <v>5558</v>
+        <v>5.558</v>
       </c>
       <c r="M4" t="n">
-        <v>0.189559</v>
+        <v>0.1866526</v>
       </c>
       <c r="N4" t="n">
-        <v>6.2e-05</v>
+        <v>5.9e-05</v>
       </c>
     </row>
     <row r="5">
@@ -636,13 +636,13 @@
         <v>200</v>
       </c>
       <c r="D5" t="n">
-        <v>0.053915</v>
+        <v>0.052011</v>
       </c>
       <c r="E5" t="n">
         <v>1390</v>
       </c>
       <c r="F5" t="n">
-        <v>0.035076</v>
+        <v>35.04089999999999</v>
       </c>
       <c r="G5" t="n">
         <v>40</v>
@@ -651,22 +651,22 @@
         <v>20.1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.009945000000000001</v>
+        <v>9.868099999999998</v>
       </c>
       <c r="J5" t="n">
-        <v>15.2</v>
+        <v>152</v>
       </c>
       <c r="K5" t="n">
-        <v>0.263796</v>
+        <v>0.2585387</v>
       </c>
       <c r="L5" t="n">
-        <v>5560</v>
+        <v>5.56</v>
       </c>
       <c r="M5" t="n">
-        <v>0.199391</v>
+        <v>0.1943055</v>
       </c>
       <c r="N5" t="n">
-        <v>5.8e-05</v>
+        <v>5.7e-05</v>
       </c>
     </row>
     <row r="6">
@@ -680,13 +680,13 @@
         <v>250</v>
       </c>
       <c r="D6" t="n">
-        <v>0.053569</v>
+        <v>0.053634</v>
       </c>
       <c r="E6" t="n">
         <v>1390</v>
       </c>
       <c r="F6" t="n">
-        <v>0.043516</v>
+        <v>43.54539999999999</v>
       </c>
       <c r="G6" t="n">
         <v>50</v>
@@ -695,22 +695,22 @@
         <v>25.1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.012363</v>
+        <v>12.1821</v>
       </c>
       <c r="J6" t="n">
-        <v>15.6</v>
+        <v>156</v>
       </c>
       <c r="K6" t="n">
-        <v>0.30159</v>
+        <v>0.2963296000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>5562</v>
+        <v>5.562</v>
       </c>
       <c r="M6" t="n">
-        <v>0.20926</v>
+        <v>0.2047147</v>
       </c>
       <c r="N6" t="n">
-        <v>5.8e-05</v>
+        <v>5.9e-05</v>
       </c>
     </row>
     <row r="7">
@@ -724,13 +724,13 @@
         <v>300</v>
       </c>
       <c r="D7" t="n">
-        <v>0.054827</v>
+        <v>0.051654</v>
       </c>
       <c r="E7" t="n">
         <v>1390</v>
       </c>
       <c r="F7" t="n">
-        <v>0.052224</v>
+        <v>51.88159999999999</v>
       </c>
       <c r="G7" t="n">
         <v>60</v>
@@ -739,22 +739,22 @@
         <v>30.1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.014951</v>
+        <v>14.5551</v>
       </c>
       <c r="J7" t="n">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="K7" t="n">
-        <v>0.338832</v>
+        <v>0.3335766999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>5564</v>
+        <v>5.564</v>
       </c>
       <c r="M7" t="n">
-        <v>0.219167</v>
+        <v>0.213082</v>
       </c>
       <c r="N7" t="n">
-        <v>6.1e-05</v>
+        <v>5.7e-05</v>
       </c>
     </row>
     <row r="8">
@@ -768,13 +768,13 @@
         <v>350</v>
       </c>
       <c r="D8" t="n">
-        <v>0.054204</v>
+        <v>0.052206</v>
       </c>
       <c r="E8" t="n">
         <v>1390</v>
       </c>
       <c r="F8" t="n">
-        <v>0.06052</v>
+        <v>59.88709999999999</v>
       </c>
       <c r="G8" t="n">
         <v>70</v>
@@ -783,22 +783,22 @@
         <v>35.1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.017448</v>
+        <v>16.9119</v>
       </c>
       <c r="J8" t="n">
-        <v>16.4</v>
+        <v>164</v>
       </c>
       <c r="K8" t="n">
-        <v>0.37759</v>
+        <v>0.3687463000000001</v>
       </c>
       <c r="L8" t="n">
-        <v>5566</v>
+        <v>5.566</v>
       </c>
       <c r="M8" t="n">
-        <v>0.22544</v>
+        <v>0.2213518</v>
       </c>
       <c r="N8" t="n">
-        <v>5.7e-05</v>
+        <v>7.3e-05</v>
       </c>
     </row>
     <row r="9">
@@ -812,13 +812,13 @@
         <v>400</v>
       </c>
       <c r="D9" t="n">
-        <v>0.053601</v>
+        <v>0.052273</v>
       </c>
       <c r="E9" t="n">
         <v>1390</v>
       </c>
       <c r="F9" t="n">
-        <v>0.069054</v>
+        <v>67.92580000000001</v>
       </c>
       <c r="G9" t="n">
         <v>80</v>
@@ -827,22 +827,22 @@
         <v>40.1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.019735</v>
+        <v>18.8731</v>
       </c>
       <c r="J9" t="n">
-        <v>16.8</v>
+        <v>168</v>
       </c>
       <c r="K9" t="n">
-        <v>0.414003</v>
+        <v>0.4032951</v>
       </c>
       <c r="L9" t="n">
-        <v>5568</v>
+        <v>5.568</v>
       </c>
       <c r="M9" t="n">
-        <v>0.235362</v>
+        <v>0.2289381</v>
       </c>
       <c r="N9" t="n">
-        <v>5.7e-05</v>
+        <v>6.1e-05</v>
       </c>
     </row>
     <row r="10">
@@ -856,13 +856,13 @@
         <v>450</v>
       </c>
       <c r="D10" t="n">
-        <v>0.054492</v>
+        <v>0.051716</v>
       </c>
       <c r="E10" t="n">
         <v>1390</v>
       </c>
       <c r="F10" t="n">
-        <v>0.077627</v>
+        <v>76.24590000000001</v>
       </c>
       <c r="G10" t="n">
         <v>90</v>
@@ -871,22 +871,22 @@
         <v>45.1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02287</v>
+        <v>21.2678</v>
       </c>
       <c r="J10" t="n">
-        <v>17.2</v>
+        <v>172</v>
       </c>
       <c r="K10" t="n">
-        <v>0.452297</v>
+        <v>0.4367034</v>
       </c>
       <c r="L10" t="n">
-        <v>5570</v>
+        <v>5.57</v>
       </c>
       <c r="M10" t="n">
-        <v>0.246277</v>
+        <v>0.2356118</v>
       </c>
       <c r="N10" t="n">
-        <v>5.7e-05</v>
+        <v>5.9e-05</v>
       </c>
     </row>
     <row r="11">
@@ -900,13 +900,13 @@
         <v>500</v>
       </c>
       <c r="D11" t="n">
-        <v>0.054119</v>
+        <v>0.05131</v>
       </c>
       <c r="E11" t="n">
         <v>1390</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08592</v>
+        <v>84.66660000000002</v>
       </c>
       <c r="G11" t="n">
         <v>100</v>
@@ -915,22 +915,22 @@
         <v>50.1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.024983</v>
+        <v>23.5857</v>
       </c>
       <c r="J11" t="n">
-        <v>17.6</v>
+        <v>176</v>
       </c>
       <c r="K11" t="n">
-        <v>0.489629</v>
+        <v>0.4721851000000001</v>
       </c>
       <c r="L11" t="n">
-        <v>5572</v>
+        <v>5.572</v>
       </c>
       <c r="M11" t="n">
-        <v>0.255794</v>
+        <v>0.2447571</v>
       </c>
       <c r="N11" t="n">
-        <v>6.600000000000001e-05</v>
+        <v>6.1e-05</v>
       </c>
     </row>
     <row r="12">
@@ -944,13 +944,13 @@
         <v>550</v>
       </c>
       <c r="D12" t="n">
-        <v>0.053712</v>
+        <v>0.051653</v>
       </c>
       <c r="E12" t="n">
         <v>1390</v>
       </c>
       <c r="F12" t="n">
-        <v>0.09400600000000001</v>
+        <v>92.762</v>
       </c>
       <c r="G12" t="n">
         <v>110</v>
@@ -959,22 +959,22 @@
         <v>55.1</v>
       </c>
       <c r="I12" t="n">
-        <v>0.02686</v>
+        <v>25.8162</v>
       </c>
       <c r="J12" t="n">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="K12" t="n">
-        <v>0.527228</v>
+        <v>0.5060454999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>5574</v>
+        <v>5.574</v>
       </c>
       <c r="M12" t="n">
-        <v>0.263933</v>
+        <v>0.2544194</v>
       </c>
       <c r="N12" t="n">
-        <v>0.000109</v>
+        <v>6.1e-05</v>
       </c>
     </row>
     <row r="13">
@@ -988,13 +988,13 @@
         <v>600</v>
       </c>
       <c r="D13" t="n">
-        <v>0.054303</v>
+        <v>0.052256</v>
       </c>
       <c r="E13" t="n">
         <v>1390</v>
       </c>
       <c r="F13" t="n">
-        <v>0.102987</v>
+        <v>101.3105</v>
       </c>
       <c r="G13" t="n">
         <v>120</v>
@@ -1003,22 +1003,22 @@
         <v>60.1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.029186</v>
+        <v>28.2899</v>
       </c>
       <c r="J13" t="n">
-        <v>18.4</v>
+        <v>184</v>
       </c>
       <c r="K13" t="n">
-        <v>0.56447</v>
+        <v>0.5420174</v>
       </c>
       <c r="L13" t="n">
-        <v>5576</v>
+        <v>5.576</v>
       </c>
       <c r="M13" t="n">
-        <v>0.272043</v>
+        <v>0.2631567</v>
       </c>
       <c r="N13" t="n">
-        <v>6.4e-05</v>
+        <v>6.1e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1032,13 +1032,13 @@
         <v>650</v>
       </c>
       <c r="D14" t="n">
-        <v>0.053443</v>
+        <v>0.051416</v>
       </c>
       <c r="E14" t="n">
         <v>1390</v>
       </c>
       <c r="F14" t="n">
-        <v>0.111902</v>
+        <v>109.1167</v>
       </c>
       <c r="G14" t="n">
         <v>130</v>
@@ -1047,22 +1047,22 @@
         <v>65.09999999999999</v>
       </c>
       <c r="I14" t="n">
-        <v>0.031828</v>
+        <v>30.3644</v>
       </c>
       <c r="J14" t="n">
-        <v>18.8</v>
+        <v>188</v>
       </c>
       <c r="K14" t="n">
-        <v>0.598623</v>
+        <v>0.5823302</v>
       </c>
       <c r="L14" t="n">
-        <v>5578</v>
+        <v>5.578</v>
       </c>
       <c r="M14" t="n">
-        <v>0.279054</v>
+        <v>0.2733833</v>
       </c>
       <c r="N14" t="n">
-        <v>7.1e-05</v>
+        <v>6.600000000000001e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1076,13 +1076,13 @@
         <v>700</v>
       </c>
       <c r="D15" t="n">
-        <v>0.056002</v>
+        <v>0.051388</v>
       </c>
       <c r="E15" t="n">
         <v>1390</v>
       </c>
       <c r="F15" t="n">
-        <v>0.12056</v>
+        <v>117.231</v>
       </c>
       <c r="G15" t="n">
         <v>140</v>
@@ -1091,22 +1091,22 @@
         <v>70.09999999999999</v>
       </c>
       <c r="I15" t="n">
-        <v>0.034123</v>
+        <v>32.6972</v>
       </c>
       <c r="J15" t="n">
-        <v>19.2</v>
+        <v>192</v>
       </c>
       <c r="K15" t="n">
-        <v>0.632675</v>
+        <v>0.6189059</v>
       </c>
       <c r="L15" t="n">
-        <v>5580</v>
+        <v>5.58</v>
       </c>
       <c r="M15" t="n">
-        <v>0.28924</v>
+        <v>0.2818899</v>
       </c>
       <c r="N15" t="n">
-        <v>7.499999999999999e-05</v>
+        <v>0.000105</v>
       </c>
     </row>
     <row r="16">
@@ -1120,13 +1120,13 @@
         <v>750</v>
       </c>
       <c r="D16" t="n">
-        <v>0.053054</v>
+        <v>0.051699</v>
       </c>
       <c r="E16" t="n">
         <v>1390</v>
       </c>
       <c r="F16" t="n">
-        <v>0.127663</v>
+        <v>125.6227</v>
       </c>
       <c r="G16" t="n">
         <v>150</v>
@@ -1135,22 +1135,22 @@
         <v>75.09999999999999</v>
       </c>
       <c r="I16" t="n">
-        <v>0.035978</v>
+        <v>35.0088</v>
       </c>
       <c r="J16" t="n">
-        <v>19.6</v>
+        <v>196</v>
       </c>
       <c r="K16" t="n">
-        <v>0.669941</v>
+        <v>0.6548914</v>
       </c>
       <c r="L16" t="n">
-        <v>5582</v>
+        <v>5.582</v>
       </c>
       <c r="M16" t="n">
-        <v>0.297546</v>
+        <v>0.2901717</v>
       </c>
       <c r="N16" t="n">
-        <v>6.8e-05</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1164,13 +1164,13 @@
         <v>800</v>
       </c>
       <c r="D17" t="n">
-        <v>0.054469</v>
+        <v>0.0523</v>
       </c>
       <c r="E17" t="n">
         <v>1390</v>
       </c>
       <c r="F17" t="n">
-        <v>0.135853</v>
+        <v>133.3715</v>
       </c>
       <c r="G17" t="n">
         <v>160</v>
@@ -1179,22 +1179,22 @@
         <v>80.09999999999999</v>
       </c>
       <c r="I17" t="n">
-        <v>0.038693</v>
+        <v>37.29430000000001</v>
       </c>
       <c r="J17" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="K17" t="n">
-        <v>0.705227</v>
+        <v>0.6914001</v>
       </c>
       <c r="L17" t="n">
-        <v>5584</v>
+        <v>5.584</v>
       </c>
       <c r="M17" t="n">
-        <v>0.305146</v>
+        <v>0.2981141</v>
       </c>
       <c r="N17" t="n">
-        <v>6.600000000000001e-05</v>
+        <v>8.899999999999999e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1208,13 +1208,13 @@
         <v>850</v>
       </c>
       <c r="D18" t="n">
-        <v>0.054111</v>
+        <v>0.05193</v>
       </c>
       <c r="E18" t="n">
         <v>1390</v>
       </c>
       <c r="F18" t="n">
-        <v>0.143593</v>
+        <v>142.0459</v>
       </c>
       <c r="G18" t="n">
         <v>170</v>
@@ -1223,22 +1223,22 @@
         <v>85.09999999999999</v>
       </c>
       <c r="I18" t="n">
-        <v>0.03996</v>
+        <v>39.67</v>
       </c>
       <c r="J18" t="n">
-        <v>20.4</v>
+        <v>204</v>
       </c>
       <c r="K18" t="n">
-        <v>0.743545</v>
+        <v>0.7265518999999999</v>
       </c>
       <c r="L18" t="n">
-        <v>5586</v>
+        <v>5.586</v>
       </c>
       <c r="M18" t="n">
-        <v>0.315617</v>
+        <v>0.3058778</v>
       </c>
       <c r="N18" t="n">
-        <v>7.4e-05</v>
+        <v>6.499999999999999e-05</v>
       </c>
     </row>
     <row r="19">
@@ -1252,13 +1252,13 @@
         <v>900</v>
       </c>
       <c r="D19" t="n">
-        <v>0.054157</v>
+        <v>0.051423</v>
       </c>
       <c r="E19" t="n">
         <v>1390</v>
       </c>
       <c r="F19" t="n">
-        <v>0.154444</v>
+        <v>150.9115</v>
       </c>
       <c r="G19" t="n">
         <v>180</v>
@@ -1267,19 +1267,19 @@
         <v>90.09999999999999</v>
       </c>
       <c r="I19" t="n">
-        <v>0.043219</v>
+        <v>41.7537</v>
       </c>
       <c r="J19" t="n">
-        <v>20.8</v>
+        <v>208</v>
       </c>
       <c r="K19" t="n">
-        <v>0.7792559999999999</v>
+        <v>0.7630923000000001</v>
       </c>
       <c r="L19" t="n">
-        <v>5588</v>
+        <v>5.588</v>
       </c>
       <c r="M19" t="n">
-        <v>0.323774</v>
+        <v>0.3158104</v>
       </c>
       <c r="N19" t="n">
         <v>6.7e-05</v>
@@ -1296,13 +1296,13 @@
         <v>950</v>
       </c>
       <c r="D20" t="n">
-        <v>0.053809</v>
+        <v>0.051081</v>
       </c>
       <c r="E20" t="n">
         <v>1390</v>
       </c>
       <c r="F20" t="n">
-        <v>0.16055</v>
+        <v>158.3252</v>
       </c>
       <c r="G20" t="n">
         <v>190</v>
@@ -1311,22 +1311,22 @@
         <v>95.09999999999999</v>
       </c>
       <c r="I20" t="n">
-        <v>0.045074</v>
+        <v>44.2044</v>
       </c>
       <c r="J20" t="n">
-        <v>21.2</v>
+        <v>212</v>
       </c>
       <c r="K20" t="n">
-        <v>0.812842</v>
+        <v>0.7970005</v>
       </c>
       <c r="L20" t="n">
-        <v>5590</v>
+        <v>5.59</v>
       </c>
       <c r="M20" t="n">
-        <v>0.33307</v>
+        <v>0.3252923</v>
       </c>
       <c r="N20" t="n">
-        <v>7.7e-05</v>
+        <v>6.499999999999999e-05</v>
       </c>
     </row>
     <row r="21">
@@ -1340,13 +1340,13 @@
         <v>1000</v>
       </c>
       <c r="D21" t="n">
-        <v>0.055265</v>
+        <v>0.051901</v>
       </c>
       <c r="E21" t="n">
         <v>1390</v>
       </c>
       <c r="F21" t="n">
-        <v>0.172566</v>
+        <v>167.0069</v>
       </c>
       <c r="G21" t="n">
         <v>200</v>
@@ -1355,22 +1355,22 @@
         <v>100.1</v>
       </c>
       <c r="I21" t="n">
-        <v>0.046344</v>
+        <v>46.2703</v>
       </c>
       <c r="J21" t="n">
-        <v>21.6</v>
+        <v>216</v>
       </c>
       <c r="K21" t="n">
-        <v>0.849146</v>
+        <v>0.8357794000000001</v>
       </c>
       <c r="L21" t="n">
-        <v>5592</v>
+        <v>5.592</v>
       </c>
       <c r="M21" t="n">
-        <v>0.341354</v>
+        <v>0.3347911</v>
       </c>
       <c r="N21" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>6.8e-05</v>
       </c>
     </row>
     <row r="22">
@@ -1384,13 +1384,13 @@
         <v>1050</v>
       </c>
       <c r="D22" t="n">
-        <v>0.056827</v>
+        <v>0.050771</v>
       </c>
       <c r="E22" t="n">
         <v>1390</v>
       </c>
       <c r="F22" t="n">
-        <v>0.180252</v>
+        <v>175.1129</v>
       </c>
       <c r="G22" t="n">
         <v>210</v>
@@ -1399,22 +1399,22 @@
         <v>105.1</v>
       </c>
       <c r="I22" t="n">
-        <v>0.052093</v>
+        <v>48.5286</v>
       </c>
       <c r="J22" t="n">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8844340000000001</v>
+        <v>0.8714166000000001</v>
       </c>
       <c r="L22" t="n">
-        <v>5594</v>
+        <v>5.594</v>
       </c>
       <c r="M22" t="n">
-        <v>0.34961</v>
+        <v>0.3431711</v>
       </c>
       <c r="N22" t="n">
-        <v>0.000127</v>
+        <v>0.000109</v>
       </c>
     </row>
     <row r="23">
@@ -1428,13 +1428,13 @@
         <v>1100</v>
       </c>
       <c r="D23" t="n">
-        <v>0.061529</v>
+        <v>0.051945</v>
       </c>
       <c r="E23" t="n">
         <v>1390</v>
       </c>
       <c r="F23" t="n">
-        <v>0.19318</v>
+        <v>183.2457</v>
       </c>
       <c r="G23" t="n">
         <v>220</v>
@@ -1443,22 +1443,22 @@
         <v>110.1</v>
       </c>
       <c r="I23" t="n">
-        <v>0.05709</v>
+        <v>51.0066</v>
       </c>
       <c r="J23" t="n">
-        <v>22.4</v>
+        <v>224</v>
       </c>
       <c r="K23" t="n">
-        <v>0.982032</v>
+        <v>0.9051252000000002</v>
       </c>
       <c r="L23" t="n">
-        <v>5596</v>
+        <v>5.596</v>
       </c>
       <c r="M23" t="n">
-        <v>0.378613</v>
+        <v>0.3510204</v>
       </c>
       <c r="N23" t="n">
-        <v>0.000105</v>
+        <v>6.9e-05</v>
       </c>
     </row>
     <row r="24">
@@ -1472,13 +1472,13 @@
         <v>1150</v>
       </c>
       <c r="D24" t="n">
-        <v>0.057594</v>
+        <v>0.050872</v>
       </c>
       <c r="E24" t="n">
         <v>1390</v>
       </c>
       <c r="F24" t="n">
-        <v>0.197185</v>
+        <v>191.6057</v>
       </c>
       <c r="G24" t="n">
         <v>230</v>
@@ -1487,22 +1487,22 @@
         <v>115.1</v>
       </c>
       <c r="I24" t="n">
-        <v>0.054939</v>
+        <v>53.2388</v>
       </c>
       <c r="J24" t="n">
-        <v>22.8</v>
+        <v>228</v>
       </c>
       <c r="K24" t="n">
-        <v>0.955493</v>
+        <v>0.9442529000000001</v>
       </c>
       <c r="L24" t="n">
-        <v>5598</v>
+        <v>5.598</v>
       </c>
       <c r="M24" t="n">
-        <v>0.365707</v>
+        <v>0.3620467</v>
       </c>
       <c r="N24" t="n">
-        <v>7.1e-05</v>
+        <v>6.7e-05</v>
       </c>
     </row>
     <row r="25">
@@ -1516,13 +1516,13 @@
         <v>1200</v>
       </c>
       <c r="D25" t="n">
-        <v>0.056834</v>
+        <v>0.052088</v>
       </c>
       <c r="E25" t="n">
         <v>1390</v>
       </c>
       <c r="F25" t="n">
-        <v>0.205761</v>
+        <v>199.8202</v>
       </c>
       <c r="G25" t="n">
         <v>240</v>
@@ -1531,22 +1531,22 @@
         <v>120.1</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0565</v>
+        <v>55.41459999999999</v>
       </c>
       <c r="J25" t="n">
-        <v>23.2</v>
+        <v>232</v>
       </c>
       <c r="K25" t="n">
-        <v>1.004384</v>
+        <v>0.9767288000000001</v>
       </c>
       <c r="L25" t="n">
-        <v>5600</v>
+        <v>5.6</v>
       </c>
       <c r="M25" t="n">
-        <v>0.384931</v>
+        <v>0.3689977999999999</v>
       </c>
       <c r="N25" t="n">
-        <v>0.000117</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="26">
@@ -1560,13 +1560,13 @@
         <v>1250</v>
       </c>
       <c r="D26" t="n">
-        <v>0.057701</v>
+        <v>0.052318</v>
       </c>
       <c r="E26" t="n">
         <v>1390</v>
       </c>
       <c r="F26" t="n">
-        <v>0.214577</v>
+        <v>208.1906</v>
       </c>
       <c r="G26" t="n">
         <v>250</v>
@@ -1575,22 +1575,22 @@
         <v>125.1</v>
       </c>
       <c r="I26" t="n">
-        <v>0.061494</v>
+        <v>57.9474</v>
       </c>
       <c r="J26" t="n">
-        <v>23.6</v>
+        <v>236</v>
       </c>
       <c r="K26" t="n">
-        <v>1.055081</v>
+        <v>1.0138167</v>
       </c>
       <c r="L26" t="n">
-        <v>5602</v>
+        <v>5.602</v>
       </c>
       <c r="M26" t="n">
-        <v>0.393284</v>
+        <v>0.3777181</v>
       </c>
       <c r="N26" t="n">
-        <v>0.00014</v>
+        <v>7.1e-05</v>
       </c>
     </row>
     <row r="27">
@@ -1604,13 +1604,13 @@
         <v>1300</v>
       </c>
       <c r="D27" t="n">
-        <v>0.058032</v>
+        <v>0.050514</v>
       </c>
       <c r="E27" t="n">
         <v>1390</v>
       </c>
       <c r="F27" t="n">
-        <v>0.223738</v>
+        <v>215.1766</v>
       </c>
       <c r="G27" t="n">
         <v>260</v>
@@ -1619,22 +1619,22 @@
         <v>130.1</v>
       </c>
       <c r="I27" t="n">
-        <v>0.06371300000000001</v>
+        <v>60.2739</v>
       </c>
       <c r="J27" t="n">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="K27" t="n">
-        <v>1.09012</v>
+        <v>1.0490257</v>
       </c>
       <c r="L27" t="n">
-        <v>5604</v>
+        <v>5.604</v>
       </c>
       <c r="M27" t="n">
-        <v>0.402774</v>
+        <v>0.3883579</v>
       </c>
       <c r="N27" t="n">
-        <v>8.8e-05</v>
+        <v>8.1e-05</v>
       </c>
     </row>
     <row r="28">
@@ -1648,13 +1648,13 @@
         <v>1350</v>
       </c>
       <c r="D28" t="n">
-        <v>0.066883</v>
+        <v>0.051753</v>
       </c>
       <c r="E28" t="n">
         <v>1390</v>
       </c>
       <c r="F28" t="n">
-        <v>0.238558</v>
+        <v>224.3901</v>
       </c>
       <c r="G28" t="n">
         <v>270</v>
@@ -1663,22 +1663,22 @@
         <v>135.1</v>
       </c>
       <c r="I28" t="n">
-        <v>0.064997</v>
+        <v>62.54339999999999</v>
       </c>
       <c r="J28" t="n">
-        <v>24.4</v>
+        <v>244</v>
       </c>
       <c r="K28" t="n">
-        <v>1.172569</v>
+        <v>1.088757</v>
       </c>
       <c r="L28" t="n">
-        <v>5606</v>
+        <v>5.606</v>
       </c>
       <c r="M28" t="n">
-        <v>0.420699</v>
+        <v>0.3949603</v>
       </c>
       <c r="N28" t="n">
-        <v>0.000144</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="29">
@@ -1692,13 +1692,13 @@
         <v>1400</v>
       </c>
       <c r="D29" t="n">
-        <v>0.058049</v>
+        <v>0.05094</v>
       </c>
       <c r="E29" t="n">
         <v>1390</v>
       </c>
       <c r="F29" t="n">
-        <v>0.241472</v>
+        <v>232.0399</v>
       </c>
       <c r="G29" t="n">
         <v>280</v>
@@ -1707,22 +1707,22 @@
         <v>140.1</v>
       </c>
       <c r="I29" t="n">
-        <v>0.068236</v>
+        <v>65.27749999999999</v>
       </c>
       <c r="J29" t="n">
-        <v>24.8</v>
+        <v>248</v>
       </c>
       <c r="K29" t="n">
-        <v>1.162706</v>
+        <v>1.1262519</v>
       </c>
       <c r="L29" t="n">
-        <v>5608</v>
+        <v>5.608</v>
       </c>
       <c r="M29" t="n">
-        <v>0.418973</v>
+        <v>0.4060505</v>
       </c>
       <c r="N29" t="n">
-        <v>0.000138</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="30">
@@ -1736,13 +1736,13 @@
         <v>1450</v>
       </c>
       <c r="D30" t="n">
-        <v>0.06281299999999999</v>
+        <v>0.052459</v>
       </c>
       <c r="E30" t="n">
         <v>1390</v>
       </c>
       <c r="F30" t="n">
-        <v>0.24828</v>
+        <v>241.4971</v>
       </c>
       <c r="G30" t="n">
         <v>290</v>
@@ -1751,22 +1751,462 @@
         <v>145.1</v>
       </c>
       <c r="I30" t="n">
-        <v>0.070868</v>
+        <v>67.12089999999998</v>
       </c>
       <c r="J30" t="n">
-        <v>25.2</v>
+        <v>252</v>
       </c>
       <c r="K30" t="n">
-        <v>1.197927</v>
+        <v>1.165281</v>
       </c>
       <c r="L30" t="n">
-        <v>5610</v>
+        <v>5.61</v>
       </c>
       <c r="M30" t="n">
-        <v>0.432606</v>
+        <v>0.4211609</v>
       </c>
       <c r="N30" t="n">
-        <v>0.000139</v>
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.054042</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F31" t="n">
+        <v>251.3277</v>
+      </c>
+      <c r="G31" t="n">
+        <v>300</v>
+      </c>
+      <c r="H31" t="n">
+        <v>150.1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>71.10250000000001</v>
+      </c>
+      <c r="J31" t="n">
+        <v>256</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1.2207208</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5.612</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.4323857</v>
+      </c>
+      <c r="N31" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1550</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.052753</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F32" t="n">
+        <v>257.7357</v>
+      </c>
+      <c r="G32" t="n">
+        <v>310</v>
+      </c>
+      <c r="H32" t="n">
+        <v>155.1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>72.1919</v>
+      </c>
+      <c r="J32" t="n">
+        <v>260</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1.2485605</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5.614</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.4513919</v>
+      </c>
+      <c r="N32" t="n">
+        <v>8.500000000000001e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.054211</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F33" t="n">
+        <v>272.0355999999999</v>
+      </c>
+      <c r="G33" t="n">
+        <v>320</v>
+      </c>
+      <c r="H33" t="n">
+        <v>160.1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>76.60579999999999</v>
+      </c>
+      <c r="J33" t="n">
+        <v>264</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1.3183701</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.616</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.4355301</v>
+      </c>
+      <c r="N33" t="n">
+        <v>7.499999999999999e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1650</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.051036</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F34" t="n">
+        <v>267.6098</v>
+      </c>
+      <c r="G34" t="n">
+        <v>330</v>
+      </c>
+      <c r="H34" t="n">
+        <v>165.1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>75.2291</v>
+      </c>
+      <c r="J34" t="n">
+        <v>268</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1.2869503</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5.618</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.4457908</v>
+      </c>
+      <c r="N34" t="n">
+        <v>7.2e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.051974</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F35" t="n">
+        <v>275.8148</v>
+      </c>
+      <c r="G35" t="n">
+        <v>340</v>
+      </c>
+      <c r="H35" t="n">
+        <v>170.1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>77.88770000000001</v>
+      </c>
+      <c r="J35" t="n">
+        <v>272</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1.330494</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.4520981</v>
+      </c>
+      <c r="N35" t="n">
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1750</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.051777</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F36" t="n">
+        <v>284.9892</v>
+      </c>
+      <c r="G36" t="n">
+        <v>350</v>
+      </c>
+      <c r="H36" t="n">
+        <v>175.1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>80.37480000000001</v>
+      </c>
+      <c r="J36" t="n">
+        <v>276</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1.3813288</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5.622</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.4779692</v>
+      </c>
+      <c r="N36" t="n">
+        <v>7.8e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.05289</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F37" t="n">
+        <v>302.4467</v>
+      </c>
+      <c r="G37" t="n">
+        <v>360</v>
+      </c>
+      <c r="H37" t="n">
+        <v>180.1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>83.85169999999999</v>
+      </c>
+      <c r="J37" t="n">
+        <v>280</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1.4514284</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5.624</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.4873145</v>
+      </c>
+      <c r="N37" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1850</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.053148</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F38" t="n">
+        <v>306.6689</v>
+      </c>
+      <c r="G38" t="n">
+        <v>370</v>
+      </c>
+      <c r="H38" t="n">
+        <v>185.1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>86.2364</v>
+      </c>
+      <c r="J38" t="n">
+        <v>284</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1.4891059</v>
+      </c>
+      <c r="L38" t="n">
+        <v>5.626</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.5047622999999999</v>
+      </c>
+      <c r="N38" t="n">
+        <v>7.9e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1900</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.054988</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F39" t="n">
+        <v>321.8945</v>
+      </c>
+      <c r="G39" t="n">
+        <v>380</v>
+      </c>
+      <c r="H39" t="n">
+        <v>190.1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>90.79689999999999</v>
+      </c>
+      <c r="J39" t="n">
+        <v>288</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1.5477549</v>
+      </c>
+      <c r="L39" t="n">
+        <v>5.628</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.5166873000000001</v>
+      </c>
+      <c r="N39" t="n">
+        <v>8.3e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1950</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.054975</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F40" t="n">
+        <v>329.825</v>
+      </c>
+      <c r="G40" t="n">
+        <v>390</v>
+      </c>
+      <c r="H40" t="n">
+        <v>195.1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>93.31369999999998</v>
+      </c>
+      <c r="J40" t="n">
+        <v>292</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1.5768658</v>
+      </c>
+      <c r="L40" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.5210357999999999</v>
+      </c>
+      <c r="N40" t="n">
+        <v>8.1e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>